<commit_message>
minor edits in data index
</commit_message>
<xml_diff>
--- a/Docs/contents/ORD_index/DummyData1_20241234_subjects.xlsx
+++ b/Docs/contents/ORD_index/DummyData1_20241234_subjects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gorka\Gitlab_crs\AFFORD_website\Docs\contents\hub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gorka\Gitlab_crs\AFFORD_website\Docs\contents\ORD_index\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38373029-E4B7-4D04-8ED9-D7DA077A3333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0BE5C1-3E39-469E-8393-C6C089CB0175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,21 +44,9 @@
     <t>Body weight [g]</t>
   </si>
   <si>
-    <t>Dilution</t>
-  </si>
-  <si>
-    <t>Concentration</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
     <t>1.5x</t>
   </si>
   <si>
-    <t>Female</t>
-  </si>
-  <si>
     <t>1x</t>
   </si>
   <si>
@@ -189,6 +177,18 @@
   </si>
   <si>
     <t>subjID</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Conc</t>
+  </si>
+  <si>
+    <t>Dilut</t>
   </si>
 </sst>
 </file>
@@ -557,7 +557,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,14 +567,14 @@
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
     <col min="8" max="8" width="19.7109375" customWidth="1"/>
     <col min="9" max="9" width="20.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -583,30 +583,30 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="C2">
         <v>27.5</v>
@@ -615,10 +615,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G2">
         <v>0.25</v>
@@ -632,10 +632,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="C3">
         <v>26.6</v>
@@ -644,10 +644,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G3">
         <v>0.5</v>
@@ -661,10 +661,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="C4">
         <v>27.5</v>
@@ -673,10 +673,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G4">
         <v>0.1</v>
@@ -690,10 +690,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="C5">
         <v>20.2</v>
@@ -702,10 +702,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G5">
         <v>0.5</v>
@@ -719,10 +719,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C6">
         <v>20.2</v>
@@ -731,10 +731,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G6">
         <v>0.5</v>
@@ -748,10 +748,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="C7">
         <v>20.3</v>
@@ -760,10 +760,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G7">
         <v>0.5</v>
@@ -777,10 +777,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="C8">
         <v>26.4</v>
@@ -789,10 +789,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E8" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G8">
         <v>0.1</v>
@@ -806,10 +806,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="C9">
         <v>24.6</v>
@@ -818,10 +818,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G9">
         <v>0.25</v>
@@ -832,10 +832,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="C10">
         <v>26.8</v>
@@ -844,10 +844,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G10">
         <v>0.25</v>
@@ -861,10 +861,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C11">
         <v>25.7</v>
@@ -873,10 +873,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G11">
         <v>0.5</v>
@@ -890,10 +890,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="C12">
         <v>24.4</v>
@@ -902,10 +902,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G12">
         <v>0.5</v>
@@ -919,10 +919,10 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="C13">
         <v>25.3</v>
@@ -931,10 +931,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E13" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G13">
         <v>0.5</v>
@@ -948,10 +948,10 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C14">
         <v>24.7</v>
@@ -960,10 +960,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G14">
         <v>0.1</v>
@@ -977,10 +977,10 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C15">
         <v>27</v>
@@ -989,10 +989,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E15" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G15">
         <v>0.1</v>
@@ -1006,10 +1006,10 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C16">
         <v>24</v>
@@ -1018,10 +1018,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E16" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G16">
         <v>0.25</v>
@@ -1035,10 +1035,10 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="C17">
         <v>25.8</v>
@@ -1047,10 +1047,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E17" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F17" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G17">
         <v>0.25</v>
@@ -1064,10 +1064,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C18">
         <v>26.4</v>
@@ -1076,10 +1076,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E18" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G18">
         <v>0.25</v>
@@ -1091,10 +1091,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="C19">
         <v>26.6</v>
@@ -1103,10 +1103,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E19" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G19">
         <v>0.25</v>
@@ -1120,10 +1120,10 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C20">
         <v>26.9</v>
@@ -1132,10 +1132,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F20" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G20">
         <v>0.5</v>
@@ -1149,10 +1149,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C21">
         <v>26.2</v>
@@ -1161,10 +1161,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E21" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F21" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G21">
         <v>0.25</v>
@@ -1178,10 +1178,10 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C22">
         <v>21</v>
@@ -1190,10 +1190,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E22" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F22" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G22">
         <v>0.5</v>
@@ -1207,10 +1207,10 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="C23">
         <v>19.5</v>
@@ -1219,10 +1219,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E23" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F23" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G23">
         <v>0.1</v>
@@ -1236,10 +1236,10 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="C24">
         <v>19.600000000000001</v>
@@ -1248,10 +1248,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E24" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F24" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G24">
         <v>0.1</v>
@@ -1265,10 +1265,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="C25">
         <v>19.559999999999999</v>
@@ -1277,10 +1277,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E25" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F25" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G25">
         <v>0.5</v>
@@ -1294,10 +1294,10 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C26">
         <v>19.63</v>
@@ -1306,10 +1306,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E26" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F26" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G26">
         <v>0.25</v>
@@ -1323,10 +1323,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C27">
         <v>19.71</v>
@@ -1335,10 +1335,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F27" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G27">
         <v>0.5</v>
@@ -1352,10 +1352,10 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C28">
         <v>19.2</v>
@@ -1364,10 +1364,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E28" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F28" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G28">
         <v>0.25</v>
@@ -1381,10 +1381,10 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C29">
         <v>20.2</v>
@@ -1393,10 +1393,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E29" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F29" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G29">
         <v>0.5</v>
@@ -1410,10 +1410,10 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C30">
         <v>18.600000000000001</v>
@@ -1422,10 +1422,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E30" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F30" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G30">
         <v>0.1</v>
@@ -1439,10 +1439,10 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C31">
         <v>19.03</v>
@@ -1451,10 +1451,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E31" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F31" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G31">
         <v>0.25</v>
@@ -1468,10 +1468,10 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="C32">
         <v>20.5</v>
@@ -1480,10 +1480,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E32" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F32" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G32">
         <v>0.25</v>
@@ -1497,10 +1497,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="C33">
         <v>20.2</v>
@@ -1509,10 +1509,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E33" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F33" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G33">
         <v>0.1</v>
@@ -1526,10 +1526,10 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C34">
         <v>21.2</v>
@@ -1538,10 +1538,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E34" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F34" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G34">
         <v>0.25</v>
@@ -1555,10 +1555,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C35">
         <v>19.21</v>
@@ -1567,10 +1567,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E35" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F35" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G35">
         <v>0.1</v>

</xml_diff>